<commit_message>
first push through teaming
</commit_message>
<xml_diff>
--- a/sp2025/teams/teams_clean.xlsx
+++ b/sp2025/teams/teams_clean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,3054 +474,3678 @@
           <t>partner_3_vid</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>team_size</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Abrar Rahman</t>
+          <t>Jacob Stephens</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>141082</v>
+        <v>185526</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>V01039276</t>
+          <t>V01070745</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fulcrum</t>
+          <t>Big Stink</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Francisco Meersohn</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>V00833042</t>
-        </is>
-      </c>
+          <t>Its Just Me</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alina Minor</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>190345</v>
-      </c>
+          <t>Austin Glass</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>V00905490</t>
+          <t>V00280987</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Warrior of Bytes</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Tyler Sapp</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>V00405652</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ronald Menendez</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>V01093990</t>
-        </is>
+          <t>ag</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Amaris Davis</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>119089</v>
-      </c>
+          <t>Ahmed Salih</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>V01030967</t>
+          <t>V00994293</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Schema Squad</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Braeden Ferguson</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>V00950948</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Jeremiah Robert</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>V01016884</t>
-        </is>
+          <t>as</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Amy Bottu</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>71251</v>
-      </c>
+          <t>Andre Smith</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>V00995688</t>
+          <t>V00993317</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Relational Rebels</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Kaleb Henderson</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>V00986435</t>
-        </is>
-      </c>
+          <t>asm</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Angela Pantigozo-Cuellar</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>113623</v>
-      </c>
+          <t>Di-Huy Tran</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>V01025475</t>
+          <t>V01045876</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>a^2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Arya Nalavade</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>V00986870</t>
-        </is>
-      </c>
+          <t>dt</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Annika Govil</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>91983</v>
-      </c>
+          <t>Marcio Tejeda</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>V01006111</t>
+          <t>V00959413</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Monkey Munchers</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Arnav Mohapatra</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>V01016443</t>
-        </is>
-      </c>
+          <t>mt</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Arnav Mohapatra</t>
+          <t>Nehemiah Akeredolu</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>105726</v>
+        <v>121176</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>V01016443</t>
+          <t>V01029185</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Monkey Munchers</t>
+          <t>na</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Annika Govil</t>
+          <t>Mohamed Elnafe</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>V01006111</t>
+          <t>VUNKNOWN</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Arya Nalavade</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>62388</v>
-      </c>
+          <t>Smeetha James</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>V00986870</t>
+          <t>V00980840</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>A Squared</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Ang Pantigozo-Cuellar</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>V01025475</t>
-        </is>
-      </c>
+          <t>sj</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ayush Upadhyay</t>
+          <t>Angela Pantigozo-Cuellar</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>111177</v>
+        <v>113623</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>V01022947</t>
+          <t>V01025475</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>The Triangles</t>
+          <t>A-squared</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Kannan</t>
+          <t>Arya Nalavade</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>V00976988</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Christopher</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>V01066649</t>
-        </is>
+          <t>V00986870</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Benhi Biguvu</t>
+          <t>Arya Nalavade</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>207977</v>
+        <v>62388</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>V01085590</t>
+          <t>V00986870</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Team Crusaders</t>
+          <t>A-squared</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Hunny Biguvu</t>
+          <t>Ang Pantigozo-Cuellar</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>V-01085673</t>
+          <t>V01025475</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bilal Othman</t>
+          <t>Ismail Jalil</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>182991</v>
+        <v>135814</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>V01069418</t>
+          <t>V01035856</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Cloud Navigators</t>
+          <t>Binary Brains</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Sameer Ali Dhanaliwala</t>
+          <t>Rayan maazouz</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>V01011114</t>
+          <t>V01071257</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bryce Strobel</t>
+          <t>Rayan Maazouz</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>136006</v>
+        <v>180405</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>V01035449</t>
+          <t>V01071257</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bryce Strobel</t>
+          <t>Binary Brains</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Emily Thompson</t>
+          <t>Ismail Jalil</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>V00937636</t>
+          <t>V01035856</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Carlos Colon</t>
+          <t>Leiliani Clark</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>133735</v>
+        <v>103565</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>V01033875</t>
+          <t>V01013390</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Pixel Pioneers</t>
+          <t>Bookworms</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Seyi Adepoju</t>
+          <t>Trinitey Tran</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>V01011000</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Yasin Yahaya</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>V01017085</t>
-        </is>
+          <t>V00981869</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carolyn Dang</t>
+          <t>Trinitey Tran</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>118372</v>
+        <v>65925</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>V01030659</t>
+          <t>V00981869</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CamboViet</t>
+          <t>Bookworms</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Theramesh Hay</t>
+          <t>Leiliani Clark</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>01012075</t>
+          <t>V01013390</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cassidy Bohn</t>
+          <t>Kwame Mensah</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>127641</v>
+        <v>68671</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>V00886655</t>
+          <t>V00990676</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>DataTrio</t>
+          <t>Buff and Bumble</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Isha Malik</t>
+          <t>Quinn Rentz</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>00977062</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Mack Hicks</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>01027708</t>
-        </is>
+          <t>V00771633</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chris Williams</t>
+          <t>Quinn Rentz</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>104931</v>
+        <v>227000</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>V01002391</t>
+          <t>V00771633</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Millionaire Minions</t>
+          <t>Buff and Bumble</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Mohamed Elnafe</t>
+          <t>Kwame Mensah</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>V00977508</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Mark Jeffery</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>V01011215</t>
-        </is>
+          <t>V00990676</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Christopher Chavez</t>
+          <t>Lauren Mack</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>111156</v>
+        <v>105397</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>V01002094</t>
+          <t>V01017234</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Database FC</t>
+          <t>Byte Sized Bandits</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Rayan Khan</t>
+          <t>Lexus Wilkinson</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>V01029314</t>
+          <t>V01030620</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Christopher Lee</t>
+          <t>Lexus Wilkinson</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>177512</v>
+        <v>118463</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>V01066649</t>
+          <t>V01030620</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>The Triangles</t>
+          <t>Byte Sized Bandits</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Kannan Venkateswaran</t>
+          <t>Lauren Mack</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>V00976988</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Ayush Upadhyay</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>V01022947</t>
-        </is>
+          <t>V01017234</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Christopher Torres</t>
+          <t>Carolyn Dang</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>196599</v>
+        <v>118372</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>V01079608</t>
+          <t>V01030659</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>408 Crew</t>
+          <t>CamboViet</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Kelechukwu Onyedeke</t>
+          <t>Theramesh Hay</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>V00916901</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Lindsey Marandina</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>V00943736</t>
-        </is>
+          <t>V01012075</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Connor Fair</t>
+          <t>Theramesh Hay</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>207306</v>
+        <v>101070</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>V01086339</t>
+          <t>V01012075</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>G&amp;C</t>
+          <t>CamboViet</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Govan Henry</t>
+          <t>Carolyn Dang</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>V01070863</t>
+          <t>V01030659</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dave Duncan</t>
+          <t>Bilal Othman</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>73096</v>
+        <v>182991</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>V00994218</t>
+          <t>V01069418</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>the strikers</t>
+          <t>Cloud Navigators</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Mahmuda Sarker</t>
+          <t>Sameer Ali Dhanaliwala</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>V00794784</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Sagai Taylor</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>V00933178</t>
-        </is>
+          <t>V01011114</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Delaney Selb</t>
+          <t>Sameer Ali Dhanaliwala</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>100293</v>
+        <v>100773</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>V00989490</t>
+          <t>V01011114</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Data Demons</t>
+          <t>Cloud Navigators</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Jamiel Dannouf</t>
+          <t>Bilal Othman</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>V00932524</t>
+          <t>V01069418</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Devin Veasna</t>
+          <t>Kyle Luchsinger</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>122000</v>
+        <v>215980</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>V01002337</t>
+          <t>V01099968</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Goobers</t>
+          <t>Code Crusaders</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Jacob Gray</t>
+          <t>Parth Dhorajia</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>V01023755</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Jenna Essex</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>V00993775</t>
-        </is>
+          <t>V01078412</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Diego Rivera</t>
+          <t>Parth Dhorajia</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>107117</v>
+        <v>190516</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>V01017210</t>
+          <t>V01078412</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Team DC</t>
+          <t>Code Crusaders</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Caitlin</t>
+          <t>Kyle Luchsinger</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>V01013162</t>
+          <t>V01099968</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>none</t>
-        </is>
+          <t>V-</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Emily Thompson</t>
+          <t>Robert Duncan</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>38248</v>
+        <v>139735</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>V00937636</t>
+          <t>V01011950</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Monacan Chiefs</t>
+          <t>CtrlAltElite</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Bryce Strobel</t>
+          <t>Steven Acosta</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>V01035449</t>
+          <t>V00970075</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Francisco Meersohn</t>
+          <t>Steven Acosta</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>15556</v>
+        <v>87914</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>V00833042</t>
+          <t>V00970075</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Fulcrum</t>
+          <t>CtrlAltElite</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Abrar Rahman</t>
+          <t>Robert Duncan</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>V01039276</t>
+          <t>V01011950</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Govan Henry</t>
+          <t>Delaney Selb</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>208056</v>
+        <v>100293</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>V01070863</t>
+          <t>V00989490</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>G&amp;C</t>
+          <t>Data Demons</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Connor Fair</t>
+          <t>Jamiel Dannouf</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>V01086339</t>
+          <t>V00932524</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Grace Weaver</t>
+          <t>Jamiel Dannouf</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>107648</v>
+        <v>185650</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>V01020601</t>
+          <t>V00932524</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Team Awesome</t>
+          <t>Data Demons</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Ivan Georgiev Chavdarov</t>
+          <t>Delaney Selb</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>V01004140</t>
+          <t>V00989490</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Hunny Biguvu</t>
+          <t>Josh Pomeroy</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>207979</v>
+        <v>27420</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>V01085673</t>
+          <t>V00954102</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Team Crusaders</t>
+          <t>Data Dynamos</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Benhi Biguvu</t>
+          <t>Rishi Ganesh</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>V-01085590</t>
+          <t>V00988725</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Isha Malik</t>
+          <t>Rishi Ganesh</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>68040</v>
+        <v>67044</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>V00977062</t>
+          <t>V00988725</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>The Data Duo</t>
+          <t>Data Dynamos</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Mack Hicks</t>
+          <t>Joshua Pomeroy</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>V01027708</t>
+          <t>V00954102</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ismail Jalil</t>
+          <t>Jaspreet Singh</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>135814</v>
+        <v>196056</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>V01035856</t>
+          <t>V01077954</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Binary Brains</t>
+          <t>Data Legends</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Rayan maazouz</t>
+          <t>Paris Davis</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>V01071257</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+          <t>V00928241</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>NIL</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>VNIL</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ivan Chavdarov</t>
+          <t>Paris Davis</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>105472</v>
+        <v>186461</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>V01004140</t>
+          <t>V00928241</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>team awesome</t>
+          <t>Data Legends</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Grace Weaver</t>
+          <t>Jaspreet Singh</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>V01020601</t>
+          <t>V01077954</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Jacob Gray</t>
+          <t>Christopher Chavez</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>112003</v>
+        <v>111156</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>V01023755</t>
+          <t>V01002094</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Goobers</t>
+          <t>Database FC</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Devin Veasna</t>
+          <t>Rayan Khan</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>v01002337</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Jenna Essex</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>v00993775</t>
-        </is>
+          <t>V01029314</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jacob Stephens</t>
+          <t>Rayan Khan</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>185526</v>
+        <v>135320</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>V01070745</t>
+          <t>V01029314</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Big Stink</t>
+          <t>Database FC</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Its Just Me</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
+          <t>Christopher Chavez</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>V01002094</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Jae Skeete</t>
+          <t>Abrar Rahman</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>155818</v>
+        <v>141082</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>V01049546</t>
+          <t>V01039276</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Static Duo</t>
+          <t>Fulcrum</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Lauren Viado</t>
+          <t>Francisco Meersohn</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>V01014153</t>
+          <t>V00833042</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jamiel Dannouf</t>
+          <t>Francisco Meersohn</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>185650</v>
+        <v>15556</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>V00932524</t>
+          <t>V00833042</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Data Demons</t>
+          <t>Fulcrum</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Delaney Selb</t>
+          <t>Abrar Rahman</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>V00989490</t>
+          <t>V01039276</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jaspreet Singh</t>
+          <t>Connor Fair</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>196056</v>
+        <v>207306</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>V01077954</t>
+          <t>V01086339</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Data Legends</t>
+          <t>G&amp;C</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Paris Davis</t>
+          <t>Govan Henry</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>V00928241</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>NIL</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>NIL</t>
-        </is>
+          <t>V01070863</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Jenna Essex</t>
+          <t>Govan Henry</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>70116</v>
+        <v>208056</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>V00993775</t>
+          <t>V01070863</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Goobers</t>
+          <t>G&amp;C</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Jacob Gray</t>
+          <t>Connor Fair</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>V01023755</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Devin Veasna</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>V01002337</t>
-        </is>
+          <t>V01086339</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jeremiah Robert</t>
+          <t>Bryce Strobel</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>104083</v>
+        <v>136006</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>V01016884</t>
+          <t>V01035449</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Schema Squad</t>
+          <t>Monacan Chiefs</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Braedan Ferguson</t>
+          <t>Emily Thompson</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>V00950948</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Amaris Davis</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>V01030967</t>
-        </is>
+          <t>V00937636</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Jon Rutan</t>
+          <t>Emily Thompson</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>207208</v>
+        <v>38248</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>V01083844</t>
+          <t>V00937636</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Open Valve</t>
+          <t>Monacan Chiefs</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Trevor Corcoran</t>
+          <t>Bryce Strobel</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>V01006310</t>
+          <t>V01035449</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Jonathan De La Pena</t>
+          <t>Annika Govil</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>112349</v>
+        <v>91983</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>V01002115</t>
+          <t>V01006111</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Team Umizumi</t>
+          <t>Monkey Munchers</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Tiffani Arbieto</t>
+          <t>Arnav Mohapatra</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>V01022008</t>
+          <t>V01016443</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Josh Pomeroy</t>
+          <t>Arnav Mohapatra</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>27420</v>
+        <v>105726</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>V00954102</t>
+          <t>V01016443</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Data Dynamos</t>
+          <t>Monkey Munchers</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Rishi Ganesh</t>
+          <t>Annika Govil</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>V00988725</t>
+          <t>V01006111</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Kaleb Henderson</t>
+          <t>Jon Rutan</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>76074</v>
+        <v>207208</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>V00986435</t>
+          <t>V01083844</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Relational Rebels</t>
+          <t>Open Valve</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Amy Bottu</t>
+          <t>Trevor Corcoran</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>V00995688</t>
+          <t>V01006310</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
+      <c r="I44" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Kannan Venkateswaran</t>
+          <t>Trevor Corcoran</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>59415</v>
+        <v>209351</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>V00976988</t>
+          <t>V01006310</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>The Triangles</t>
+          <t>Open Valve</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Ayush Upadhyay</t>
+          <t>Jonathan Rutan</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>V01022947</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Christopher Lee</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>V01066649</t>
-        </is>
+          <t>V01083844</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Kel Raphael</t>
+          <t>Amy Bottu</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>64311</v>
+        <v>71251</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>V00975947</t>
+          <t>V00995688</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Random Word Generators</t>
+          <t>Relational Rebels</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Sage Ginther</t>
+          <t>Kaleb Henderson</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>01054676</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Naomi Boyett</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>01003278</t>
-        </is>
+          <t>V00986435</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Kelechukwu Onyedeke</t>
+          <t>Kaleb Henderson</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>25873</v>
+        <v>76074</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>V00916901</t>
+          <t>V00986435</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>408 crew</t>
+          <t>Relational Rebels</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Christopher Torres</t>
+          <t>Amy Bottu</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>V01079608</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Lindsey Marandina</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>V00943736</t>
-        </is>
+          <t>V00995688</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Kwame Mensah</t>
+          <t>Kyle Jones</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>68671</v>
+        <v>27451</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>V00990676</t>
+          <t>V00946860</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Buff and Bumble</t>
+          <t>Secondhand Friends</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Quinn Rentz</t>
+          <t>Youssef Bahloul</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>V00771633</t>
+          <t>V00971107</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Youssef Bahloul</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>59133</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>V00971107</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Secondhand Friends</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>Kyle Jones</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>27451</v>
-      </c>
-      <c r="C49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>V00946860</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Secondhand Friends</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Youssef Bahloul</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>V00971107</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Kyle Luchsinger</t>
+          <t>Jae Skeete</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>215980</v>
+        <v>155818</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>V01099968</t>
+          <t>V01049546</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Code Crusaders</t>
+          <t>Static Duo</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Parth Dhorajia</t>
+          <t>Lauren Viado</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>V01078412</t>
+          <t>V01014153</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Lauren Mack</t>
+          <t>Lauren Viado</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>105397</v>
+        <v>106768</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>V01017234</t>
+          <t>V01014153</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Byte Sized Bandits</t>
+          <t>Static Duo</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Lexus Wilkinson</t>
+          <t>Jae Skeete</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>V01030620</t>
+          <t>V01049546</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Lauren Viado</t>
+          <t>Grace Weaver</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>106768</v>
+        <v>107648</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>V01014153</t>
+          <t>V01020601</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>static duo</t>
+          <t>Team Awesome</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Jae Skeete</t>
+          <t>Ivan Georgiev Chavdarov</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>V01049546</t>
+          <t>V01004140</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Leiliani Clark</t>
+          <t>Ivan Chavdarov</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>103565</v>
+        <v>105472</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>V01013390</t>
+          <t>V01004140</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Bookworms</t>
+          <t>Team Awesome</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Trinitey Tran</t>
+          <t>Grace Weaver</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>00981869</t>
+          <t>V01020601</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
+      <c r="I53" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Lexus Wilkinson</t>
+          <t>Benhi Biguvu</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>118463</v>
+        <v>207977</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>V01030620</t>
+          <t>V01085590</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Byte Sized Bandits</t>
+          <t>Team Crusaders</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Lauren Mack</t>
+          <t>Hunny Biguvu</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>V01017234</t>
+          <t>V-01085673</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
+      <c r="I54" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Lily Winsor</t>
+          <t>Hunny Biguvu</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>71999</v>
+        <v>207979</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>V00993136</t>
+          <t>V01085673</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>The Optimizers</t>
+          <t>Team Crusaders</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Nicole Yazbeck</t>
+          <t>Benhi Biguvu</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>V01046036</t>
+          <t>V-01085590</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
+      <c r="I55" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Lindsey Marandina</t>
+          <t>Diego Rivera</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>51883</v>
+        <v>107117</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>V00943736</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr"/>
+          <t>V01017210</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Team DC</t>
+        </is>
+      </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Christopher Torres</t>
+          <t>Caitlin</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>V01079608</t>
+          <t>V01013162</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Kelechukwu Onyedeke</t>
+          <t>none</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>V00916901</t>
-        </is>
+          <t>VNONE</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mack Hicks</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>115504</v>
-      </c>
+          <t>Caitlin Berdeguez</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>V01027708</t>
+          <t>V01013162</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>DataTrio</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Isha Malik</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>V00977062</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Cassidy Bohn</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>V00886655</t>
-        </is>
+          <t>Team DC</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Mahmuda Sarker</t>
+          <t>Jonathan De La Pena</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>14274</v>
+        <v>112349</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>V00794784</t>
+          <t>V01002115</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>CMSC 408</t>
+          <t>Team UmiZumi</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sagai Taylor</t>
+          <t>Tiffani Arbieto</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>V00933178</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Dave Duncan</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>V00994218</t>
-        </is>
+          <t>V01022008</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Mark Jeffrey</t>
+          <t>Tiffani M Arbieto Arbieto</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>107852</v>
+        <v>118079</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>V01011215</t>
+          <t>V01022008</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Millionaire Minions</t>
+          <t>Team UmiZumi</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>MoHamed Elnafe</t>
+          <t>Jonathan De La Peña</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>V00977508</t>
+          <t>V01002115</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
+      <c r="I59" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Mark Wells</t>
+          <t>Lily Winsor</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>105757</v>
+        <v>71999</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>V01014035</t>
+          <t>V00993136</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Data Knights</t>
+          <t>The Optimizers</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Salil</t>
+          <t>Nicole Yazbeck</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>V01023365</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Samih</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>V01002314</t>
-        </is>
+          <t>V01046036</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mohamed Elnafe</t>
+          <t>Nicole Yazbeck</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>80703</v>
+        <v>158345</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>V00977508</t>
+          <t>V01046036</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Millionaire Minions</t>
+          <t>The Optimizers</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Mark Jeffery</t>
+          <t>Lily Winsor</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>V01011215</t>
+          <t>V00993136</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Muhammad Amjad</t>
+          <t>Christopher Torres</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>159827</v>
+        <v>196599</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>V01052051</t>
+          <t>V01079608</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Team Arceus</t>
+          <t>408 Crew</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Sriram Sathvik Vangipurpau</t>
+          <t>Kelechukwu Onyedeke</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>V01026262</t>
+          <t>V00916901</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Nima Behboudi</t>
+          <t>Lindsey Marandina</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>V01080146</t>
-        </is>
+          <t>V00943736</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Naomi Boyett</t>
+          <t>Kelechukwu Onyedeke</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>106645</v>
+        <v>25873</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>V01003278</t>
+          <t>V00916901</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Random Word Generators</t>
+          <t>408 Crew</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Sage Ginther</t>
+          <t>Christopher Torres</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>V01054676</t>
+          <t>V01079608</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Kel Raphael</t>
+          <t>Lindsey Marandina</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>V00975947</t>
-        </is>
+          <t>V00943736</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Nehemiah Akeredolu</t>
+          <t>Lindsey Marandina</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>121176</v>
+        <v>51883</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>V01029185</t>
+          <t>V00943736</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>not yet decided</t>
+          <t>408 Crew</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Mohamed Elnafe</t>
+          <t>Christopher Torres</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
+          <t>V01079608</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Kelechukwu Onyedeke</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>V00916901</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Nicole Yazbeck</t>
+          <t>Mark Wells</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>158345</v>
+        <v>105757</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>V01046036</t>
+          <t>V01014035</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>The Optimizers</t>
+          <t>Data Knights</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Lily Winsor</t>
+          <t>Salil</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>V00993136</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
+          <t>V01023365</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Samih</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>V01002314</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Nima Behboudi</t>
+          <t>Salil Chalise</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>196067</v>
+        <v>111252</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>V01080146</t>
+          <t>V01023365</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Arceus</t>
+          <t>Data Knights</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Sriram Sathvik Vangipurpau</t>
+          <t>Samih</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>V01026262</t>
+          <t>V01002314</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Muhammad Amjad</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>V01052051</t>
-        </is>
+          <t>V01014035</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Paris Davis</t>
+          <t>Samih Siddiqi</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>186461</v>
+        <v>105467</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>V00928241</t>
+          <t>V01002314</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Data Legends</t>
+          <t>Data Knights</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Jaspreet Singh</t>
+          <t>Salil</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>V01077954</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
+          <t>V01023365</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>V01014035</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Parth Dhorajia</t>
+          <t>Cassidy Bohn</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>190516</v>
+        <v>127641</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>V01078412</t>
+          <t>V00886655</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Code Crusaders</t>
+          <t>Data Trio</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Kyle Luchsinger</t>
+          <t>Isha Malik</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>V01099968</t>
+          <t>V00977062</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Mack Hicks</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
+          <t>V01027708</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Quinn Rentz</t>
+          <t>Isha Malik</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>227000</v>
+        <v>68040</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>V00771633</t>
+          <t>V00977062</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Buff and Bumble</t>
+          <t>Data Trio</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Kwame Mensah</t>
+          <t>Mack Hicks</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>V00990676</t>
+          <t>V01027708</t>
         </is>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Rayan Khan</t>
+          <t>Mack Hicks</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>135320</v>
+        <v>115504</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>V01029314</t>
+          <t>V01027708</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Database FC</t>
+          <t>Data Trio</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Christopher Chavez</t>
+          <t>Isha Malik</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>V01002094</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
+          <t>V00977062</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Cassidy Bohn</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>V00886655</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Rayan Maazouz</t>
+          <t>Carlos Colon</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>180405</v>
+        <v>133735</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>V01071257</t>
+          <t>V01033875</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Binary Brains</t>
+          <t>Entergalactic Coders</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Ismail Jalil</t>
+          <t>Seyi Adepoju</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>V01035856</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
+          <t>V01011000</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Yasin Yahaya</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>V01017085</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Rishi Ganesh</t>
+          <t>Yasin Yahaya</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>67044</v>
+        <v>108286</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>V00988725</t>
+          <t>V01017085</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Data Dynamos</t>
+          <t>Entergalactic Coders</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Joshua Pomeroy</t>
+          <t>Seyi Adepoju</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>V00954102</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
+          <t>V01011000</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Carlos Colon</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>V01033875</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Robert Duncan</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>139735</v>
-      </c>
+          <t>SeyiYash Upadhyay</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>V01011950</t>
+          <t>V01011000</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>CtrlAltElite</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Steven Acosta</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>V00970075</t>
-        </is>
-      </c>
+          <t>Entergalactic Coders</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Ronald Menendez</t>
+          <t>Devin Veasna</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>208291</v>
+        <v>122000</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>V01093990</t>
+          <t>V01002337</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Warriors of Btye</t>
+          <t>Goobers</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Tyler Sapp</t>
+          <t>Jacob Gray</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>V00405652</t>
+          <t>V01023755</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Alina Minor</t>
+          <t>Jenna Essex</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>V00905490</t>
-        </is>
+          <t>V00993775</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Sagai Taylor</t>
+          <t>Jacob Gray</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>29004</v>
+        <v>112003</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>V00933178</t>
+          <t>V01023755</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Strikers</t>
+          <t>Goobers</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Dave Duncan</t>
+          <t>Devin Veasna</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>V00994218</t>
+          <t>V01002337</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Mahmuda Sarker</t>
+          <t>Jenna Essex</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>V00794784</t>
-        </is>
+          <t>V00993775</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sage Ginther</t>
+          <t>Jenna Essex</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>177633</v>
+        <v>70116</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>V01054676</t>
+          <t>V00993775</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Random Word Generators</t>
+          <t>Goobers</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Naomi Boyett</t>
+          <t>Jacob Gray</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>V01003278</t>
+          <t>V01023755</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Kel Raphael</t>
+          <t>Devin Veasna</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>V00975947</t>
-        </is>
+          <t>V01002337</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Salil Chalise</t>
+          <t>Chris Williams</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>111252</v>
+        <v>104931</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>V01023365</t>
+          <t>V01002391</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Data Knights</t>
+          <t>Millionaire Minions</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Samih</t>
+          <t>Mohamed Elnafe</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>V01002314</t>
+          <t>V00977508</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Mark Jeffery</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>V01014035</t>
-        </is>
+          <t>V01011215</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sameer Ali Dhanaliwala</t>
+          <t>Mark Jeffrey</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>100773</v>
+        <v>107852</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>V01011114</t>
+          <t>V01011215</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Cloud Navigators</t>
+          <t>Millionaire Minions</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Bilal Othman</t>
+          <t>MoHamed Elnafe</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>V01069418</t>
+          <t>V00977508</t>
         </is>
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Samih Siddiqi</t>
+          <t>Mohamed Elnafe</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>105467</v>
+        <v>80703</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>V01002314</t>
+          <t>V00977508</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Data Knights</t>
+          <t>Millionaire Minions</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Salil</t>
+          <t>Mark Jeffery</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>V01023365</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Mark</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>V01014035</t>
-        </is>
+          <t>V01011215</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sriram Sathvik Vangipurapu</t>
+          <t>Gladys Ayanou</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>114722</v>
+        <v>172726</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>V01026262</t>
+          <t>V01062706</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Arceus</t>
+          <t>Minion</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Nima Behboudi</t>
+          <t>Katang Phuthongthiam</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>V01080146</t>
+          <t>V01033266</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Muhammad Amjad</t>
+          <t>Noah D'Souza</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>V01052051</t>
-        </is>
+          <t>V01029094</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Steven Acosta</t>
+          <t>Katang Phuthongthiam</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>87914</v>
+        <v>123421</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>V00970075</t>
+          <t>V01033266</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>CtrlAltElite</t>
+          <t>Minion</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Robert Duncan</t>
+          <t>Gladys Ayanou</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>V01011950</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
+          <t>V01062706</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Noah D’Souza</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>V0102909</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Theramesh Hay</t>
+          <t>Noah D'Souza</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>101070</v>
+        <v>125082</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>V01012075</t>
+          <t>V01029094</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>CamboViet</t>
+          <t>Minion</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Carolyn Dang</t>
+          <t>Gladys Ayanou</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>01030659</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
+          <t>V01062706</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Katang Phuthongthiam</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>V01033266</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Tiffani M Arbieto Arbieto</t>
+          <t>Kel Raphael</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>118079</v>
+        <v>64311</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>V01022008</t>
+          <t>V00975947</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Team UmiZumi</t>
+          <t>Random Word Generators</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Jonathan De La Peña</t>
+          <t>Sage Ginther</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>V01002115</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
+          <t>V01054676</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Naomi Boyett</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>V01003278</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Trevor Corcoran</t>
+          <t>Naomi Boyett</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>209351</v>
+        <v>106645</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>V01006310</t>
+          <t>V01003278</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Open Valve</t>
+          <t>Random Word Generators</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Jonathan Rutan</t>
+          <t>Sage Ginther</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>V01083844</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
+          <t>V01054676</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Kel Raphael</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>V00975947</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Trinitey Tran</t>
+          <t>Sage Ginther</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>65925</v>
+        <v>177633</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>V00981869</t>
+          <t>V01054676</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Bookworms</t>
+          <t>Random Word Generators</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Leiliani Clark</t>
+          <t>Naomi Boyett</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>01013390</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
+          <t>V01003278</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Kel Raphael</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>V00975947</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Tyler Sapp</t>
+          <t>Amaris Davis</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>8487</v>
+        <v>119089</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>V00405652</t>
+          <t>V01030967</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Warriors of Byte</t>
+          <t>Schema Squad</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Alina Minor</t>
+          <t>Braeden Ferguson</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>V00905490</t>
+          <t>V00950948</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Ronald Menendez</t>
+          <t>Jeremiah Robert</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>V01093990</t>
-        </is>
+          <t>V01016884</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Yasin Yahaya</t>
+          <t>Jeremiah Robert</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>108286</v>
+        <v>104083</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>V01017085</t>
+          <t>V01016884</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Entergalactic Coders</t>
+          <t>Schema Squad</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Seyi Adepoju</t>
+          <t>Braedan Ferguson</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>V01011000</t>
+          <t>V00950948</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Carlos Colon</t>
+          <t>Amaris Davis</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>V01033875</t>
-        </is>
+          <t>V01030967</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Youssef Bahloul</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
-        <v>59133</v>
-      </c>
+          <t>Braeden Ferguson</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>V00971107</t>
+          <t>V00950948</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Secondhand Friends</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Kyle Jones</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>V00946860</t>
-        </is>
-      </c>
+          <t>Schema Squad</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
+      <c r="I88" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Dave Duncan</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>73096</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>V00994218</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Strikers</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Mahmuda Sarker</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>V00794784</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Sagai Taylor</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>V00933178</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Mahmuda Sarker</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>14274</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>V00794784</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Strikers</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Sagai Taylor</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>V00933178</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Dave Duncan</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>V00994218</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Sagai Taylor</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>29004</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>V00933178</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Strikers</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Dave Duncan</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>V00994218</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Mahmuda Sarker</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>V00794784</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Muhammad Amjad</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>159827</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>V01052051</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Team Arceus</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Sriram Sathvik Vangipurpau</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>V01026262</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Nima Behboudi</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>V01080146</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Nima Behboudi</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>196067</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>V01080146</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Team Arceus</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Sriram Sathvik Vangipurpau</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>V01026262</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Muhammad Amjad</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>V01052051</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Sriram Sathvik Vangipurapu</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>114722</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>V01026262</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Team Arceus</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Nima Behboudi</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>V01080146</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Muhammad Amjad</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>V01052051</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Ayush Upadhyay</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>111177</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>V01022947</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>The Triangles</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Kannan</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>V00976988</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Christopher</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>V01066649</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Christopher Lee</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>177512</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>V01066649</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>The Triangles</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Kannan Venkateswaran</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>V00976988</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Ayush Upadhyay</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>V01022947</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Kannan Venkateswaran</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>59415</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>V00976988</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>The Triangles</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Ayush Upadhyay</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>V01022947</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Christopher Lee</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>V01066649</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Alina Minor</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>190345</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>V00905490</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Warriors of Bytes</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Tyler Sapp</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>V00405652</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Ronald Menendez</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>V01093990</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Ronald Menendez</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>208291</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>V01093990</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Warriors of Bytes</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Tyler Sapp</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>V00405652</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Alina Minor</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>V00905490</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Tyler Sapp</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>8487</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>V00405652</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Warriors of Bytes</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Alina Minor</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>V00905490</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Ronald Menendez</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>V01093990</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>